<commit_message>
수정: @RequestParam로 변경 in AttractionController.java
</commit_message>
<xml_diff>
--- a/enjoytrip_RESTAPI설계.xlsx
+++ b/enjoytrip_RESTAPI설계.xlsx
@@ -878,7 +878,7 @@
   <dimension ref="B2:H111"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1042,7 +1042,7 @@
       <c r="G10" s="3"/>
       <c r="H10" s="9"/>
     </row>
-    <row r="11" spans="2:8" ht="33" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B11" s="3" t="s">
         <v>64</v>
       </c>
@@ -1458,7 +1458,7 @@
       <c r="G62" s="7"/>
       <c r="H62" s="7"/>
     </row>
-    <row r="100" spans="2:7" ht="49.5" x14ac:dyDescent="0.3">
+    <row r="100" spans="2:7" ht="33" x14ac:dyDescent="0.3">
       <c r="B100" s="3" t="s">
         <v>53</v>
       </c>
@@ -1478,7 +1478,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="101" spans="2:7" ht="33" x14ac:dyDescent="0.3">
+    <row r="101" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B101" s="3" t="s">
         <v>6</v>
       </c>
@@ -1518,7 +1518,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="103" spans="2:7" ht="33" x14ac:dyDescent="0.3">
+    <row r="103" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B103" s="3" t="s">
         <v>9</v>
       </c>
@@ -1580,7 +1580,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="107" spans="2:7" ht="33" x14ac:dyDescent="0.3">
+    <row r="107" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B107" s="3" t="s">
         <v>9</v>
       </c>
@@ -1618,7 +1618,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="109" spans="2:7" ht="82.5" x14ac:dyDescent="0.3">
+    <row r="109" spans="2:7" ht="66" x14ac:dyDescent="0.3">
       <c r="B109" s="3" t="s">
         <v>10</v>
       </c>
@@ -1638,7 +1638,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="110" spans="2:7" ht="82.5" x14ac:dyDescent="0.3">
+    <row r="110" spans="2:7" ht="66" x14ac:dyDescent="0.3">
       <c r="B110" s="3" t="s">
         <v>11</v>
       </c>
@@ -1658,7 +1658,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="111" spans="2:7" ht="33" x14ac:dyDescent="0.3">
+    <row r="111" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B111" s="3" t="s">
         <v>12</v>
       </c>

</xml_diff>